<commit_message>
Fotos do osciloscópio + Excel dos transistores
IGNORAR excel dos transistores
</commit_message>
<xml_diff>
--- a/-114/Amplificadores/T3B&4A - Amplificadores operacionais.xlsx
+++ b/-114/Amplificadores/T3B&4A - Amplificadores operacionais.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAII\-114\Amplificadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751B095A-9BC4-4C0A-BA93-3BCF880ED987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E5B283-6BB1-4819-A34A-BDB0BDE1E54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8FB4B29B-C6EF-4146-BDDD-17EC50990B13}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{8FB4B29B-C6EF-4146-BDDD-17EC50990B13}"/>
   </bookViews>
   <sheets>
     <sheet name="Inversora" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
   <si>
     <r>
       <t>V</t>
@@ -414,6 +414,9 @@
   <si>
     <t>Ganho 100</t>
   </si>
+  <si>
+    <t>Valor Típico para 741</t>
+  </si>
 </sst>
 </file>
 
@@ -546,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -590,6 +593,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,7 +608,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1475,6 +1484,475 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.0022747156605423E-2"/>
+                  <c:y val="-0.13810987168270633"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Inversora!$V$15:$V$36</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Inversora!$W$15:$W$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>8.0392156862745097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2549019607843137</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5048543689320386</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0784313725490193</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5339805825242721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0961538461538458</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7572815533980588</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9514563106796112</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3495145631067968</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.7307692307692304</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2380952380952377</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.6153846153846154</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1714285714285713</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6538461538461537</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4476190476190476</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3018867924528301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0377358490566038</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.88679245283018859</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.660377358490566</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.24761904761904763</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.12307692307692307</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B9B6-4B61-BA8F-C1D390878570}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1359966063"/>
+        <c:axId val="1359962223"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1359966063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1359962223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1359962223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1359966063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2134,7 +2612,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2300,7 +2777,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3178,463 +3655,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.8721784776902888E-2"/>
-                  <c:y val="-0.2121839457567804"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Não inversora'!$T$21:$T$40</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0" formatCode="0.0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.0">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.0">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="0.0">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="0.0">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="0.0">
-                  <c:v>200</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Não inversora'!$U$21:$U$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>9.7169811320754711</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.8571428571428577</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.3809523809523814</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.8301886792452837</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.9444444444444438</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.0925925925925926</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.2129629629629628</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.657142857142857</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.2692307692307692</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.9230769230769229</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.6407766990291264</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.1923076923076921</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8846153846153846</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.638095238095238</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.2924528301886793</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.0943396226415094</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.90566037735849048</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.72380952380952379</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E9F6-4248-8A77-112C8917C8BE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="907716719"/>
-        <c:axId val="907719599"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="907716719"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="907719599"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="907719599"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="907716719"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5864,13 +5884,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>220980</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>80682</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>559440</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>170820</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>148902</xdr:rowOff>
     </xdr:to>
@@ -5894,6 +5914,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F431AFD-E1B5-6C46-8E53-A8EF82B453C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5973,42 +6029,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>231913</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>178904</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>536713</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>139148</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2725309-80F9-0BDF-586C-6EA7FE3501BA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6314,10 +6334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663C5FF8-D826-4997-ABED-6EB55FC7BB49}">
-  <dimension ref="B4:R37"/>
+  <dimension ref="B4:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView topLeftCell="C9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6331,16 +6351,16 @@
     <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="7" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="7" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -6366,7 +6386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <v>1</v>
       </c>
@@ -6395,7 +6415,7 @@
         <v>7.1421285462900941E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <v>2</v>
       </c>
@@ -6424,7 +6444,7 @@
         <v>7.1421285462900941E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
         <v>3</v>
       </c>
@@ -6453,7 +6473,7 @@
         <v>7.0007142492748559E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
         <v>4</v>
       </c>
@@ -6482,7 +6502,7 @@
         <v>6.9658093571386234E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
         <v>5</v>
       </c>
@@ -6511,7 +6531,7 @@
         <v>6.9658093571386234E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
         <v>10</v>
       </c>
@@ -6540,7 +6560,7 @@
         <v>6.9658093571386234E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
         <v>12</v>
       </c>
@@ -6569,7 +6589,7 @@
         <v>6.7962872406606367E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
         <v>14</v>
       </c>
@@ -6597,8 +6617,18 @@
         <f t="shared" si="1"/>
         <v>6.5056643457712823E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="1">
+        <f>H15*B15</f>
+        <v>122.15686274509805</v>
+      </c>
+      <c r="V15" s="13">
+        <v>16</v>
+      </c>
+      <c r="W15" s="1">
+        <v>8.0392156862745097</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
         <v>16</v>
       </c>
@@ -6626,8 +6656,18 @@
         <f t="shared" si="1"/>
         <v>6.2895994421310594E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J16" s="1">
+        <f t="shared" ref="J16:J36" si="3">H16*B16</f>
+        <v>128.62745098039215</v>
+      </c>
+      <c r="V16" s="13">
+        <v>18</v>
+      </c>
+      <c r="W16" s="1">
+        <v>7.2549019607843137</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
         <v>18</v>
       </c>
@@ -6655,8 +6695,18 @@
         <f t="shared" si="1"/>
         <v>6.0561261061220159E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J17" s="1">
+        <f t="shared" si="3"/>
+        <v>130.58823529411765</v>
+      </c>
+      <c r="V17" s="13">
+        <v>20</v>
+      </c>
+      <c r="W17" s="1">
+        <v>6.5048543689320386</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
         <v>20</v>
       </c>
@@ -6684,8 +6734,18 @@
         <f t="shared" si="1"/>
         <v>5.7910226751047761E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J18" s="1">
+        <f t="shared" si="3"/>
+        <v>130.09708737864077</v>
+      </c>
+      <c r="V18" s="13">
+        <v>22</v>
+      </c>
+      <c r="W18" s="1">
+        <v>6.0784313725490193</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
         <v>22</v>
       </c>
@@ -6713,8 +6773,18 @@
         <f t="shared" si="1"/>
         <v>5.7364949294028349E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J19" s="1">
+        <f t="shared" si="3"/>
+        <v>133.72549019607843</v>
+      </c>
+      <c r="V19" s="13">
+        <v>24</v>
+      </c>
+      <c r="W19" s="1">
+        <v>5.5339805825242721</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
         <v>24</v>
       </c>
@@ -6742,8 +6812,18 @@
         <f t="shared" si="1"/>
         <v>5.5481198414453016E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J20" s="1">
+        <f t="shared" si="3"/>
+        <v>132.81553398058253</v>
+      </c>
+      <c r="V20" s="13">
+        <v>26</v>
+      </c>
+      <c r="W20" s="1">
+        <v>5.0961538461538458</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
         <v>26</v>
       </c>
@@ -6771,6 +6851,10 @@
         <f t="shared" si="1"/>
         <v>5.3959955297377737E-2</v>
       </c>
+      <c r="J21" s="1">
+        <f t="shared" si="3"/>
+        <v>132.5</v>
+      </c>
       <c r="K21" s="2" t="s">
         <v>0</v>
       </c>
@@ -6781,18 +6865,24 @@
         <v>8</v>
       </c>
       <c r="O21" s="8">
-        <f>1.4*10^-4</f>
-        <v>1.3999999999999999E-4</v>
+        <f>1.4*10^-3</f>
+        <v>1.4E-3</v>
       </c>
       <c r="Q21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R21" s="11">
         <f>L21/O21</f>
-        <v>7142.8571428571431</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+        <v>714.28571428571433</v>
+      </c>
+      <c r="V21" s="13">
+        <v>28</v>
+      </c>
+      <c r="W21" s="1">
+        <v>4.7572815533980588</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
         <v>28</v>
       </c>
@@ -6820,6 +6910,10 @@
         <f t="shared" si="1"/>
         <v>5.3756898379145518E-2</v>
       </c>
+      <c r="J22" s="1">
+        <f t="shared" si="3"/>
+        <v>133.20388349514565</v>
+      </c>
       <c r="K22" s="2" t="s">
         <v>5</v>
       </c>
@@ -6838,10 +6932,16 @@
       </c>
       <c r="R22" s="9">
         <f>SQRT((L22/O21)^2+(O22*L21/O21^2)^2)</f>
-        <v>510.25407918289324</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+        <v>5.1517981883119752</v>
+      </c>
+      <c r="V22" s="13">
+        <v>27</v>
+      </c>
+      <c r="W22" s="1">
+        <v>4.9514563106796112</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
         <v>27</v>
       </c>
@@ -6869,15 +6969,25 @@
         <f t="shared" si="1"/>
         <v>5.4168519231575479E-2</v>
       </c>
+      <c r="J23" s="1">
+        <f t="shared" si="3"/>
+        <v>133.6893203883495</v>
+      </c>
       <c r="Q23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R23" s="10">
         <f>R22/R21*100</f>
-        <v>7.1435571085605059</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+        <v>0.7212517463636765</v>
+      </c>
+      <c r="V23" s="13">
+        <v>30</v>
+      </c>
+      <c r="W23" s="1">
+        <v>4.3495145631067968</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="13">
         <v>30</v>
       </c>
@@ -6905,15 +7015,25 @@
         <f t="shared" si="1"/>
         <v>2.1664998474279197E-2</v>
       </c>
+      <c r="J24" s="1">
+        <f t="shared" si="3"/>
+        <v>130.48543689320391</v>
+      </c>
       <c r="Q24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="R24" s="11">
         <f>(R21-R26)/R26*100</f>
-        <v>-27.483683828861494</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+        <v>-28.212491026561377</v>
+      </c>
+      <c r="V24" s="13">
+        <v>35</v>
+      </c>
+      <c r="W24" s="1">
+        <v>3.7307692307692304</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B25" s="13">
         <v>35</v>
       </c>
@@ -6941,8 +7061,18 @@
         <f t="shared" si="1"/>
         <v>1.8569545246488708E-2</v>
       </c>
-    </row>
-    <row r="26" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J25" s="1">
+        <f t="shared" si="3"/>
+        <v>130.57692307692307</v>
+      </c>
+      <c r="V25" s="13">
+        <v>40</v>
+      </c>
+      <c r="W25" s="1">
+        <v>3.2380952380952377</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="13">
         <v>40</v>
       </c>
@@ -6970,14 +7100,24 @@
         <f t="shared" si="1"/>
         <v>1.6138052923952911E-2</v>
       </c>
+      <c r="J26" s="1">
+        <f t="shared" si="3"/>
+        <v>129.52380952380952</v>
+      </c>
       <c r="Q26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="R26" s="7">
-        <v>9850</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+        <v>995</v>
+      </c>
+      <c r="V26" s="13">
+        <v>50</v>
+      </c>
+      <c r="W26" s="1">
+        <v>2.6153846153846154</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="13">
         <v>50</v>
       </c>
@@ -7005,14 +7145,24 @@
         <f t="shared" si="1"/>
         <v>1.3461741659172554E-2</v>
       </c>
+      <c r="J27" s="1">
+        <f t="shared" si="3"/>
+        <v>130.76923076923077</v>
+      </c>
       <c r="Q27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="R27" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="V27" s="13">
+        <v>60</v>
+      </c>
+      <c r="W27" s="1">
+        <v>2.1714285714285713</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B28" s="13">
         <v>60</v>
       </c>
@@ -7040,8 +7190,18 @@
         <f t="shared" si="1"/>
         <v>1.1383942664358609E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J28" s="1">
+        <f t="shared" si="3"/>
+        <v>130.28571428571428</v>
+      </c>
+      <c r="V28" s="13">
+        <v>70</v>
+      </c>
+      <c r="W28" s="1">
+        <v>1.8666666666666665</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
         <v>70</v>
       </c>
@@ -7069,8 +7229,18 @@
         <f t="shared" si="1"/>
         <v>1.0084050904297518E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J29" s="1">
+        <f t="shared" si="3"/>
+        <v>130.66666666666666</v>
+      </c>
+      <c r="V29" s="13">
+        <v>80</v>
+      </c>
+      <c r="W29" s="1">
+        <v>1.6538461538461537</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B30" s="13">
         <v>80</v>
       </c>
@@ -7098,8 +7268,18 @@
         <f t="shared" si="1"/>
         <v>9.2916749455629524E-3</v>
       </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J30" s="1">
+        <f t="shared" si="3"/>
+        <v>132.30769230769229</v>
+      </c>
+      <c r="V30" s="13">
+        <v>90</v>
+      </c>
+      <c r="W30" s="1">
+        <v>1.4476190476190476</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B31" s="13">
         <v>90</v>
       </c>
@@ -7127,8 +7307,18 @@
         <f t="shared" si="1"/>
         <v>8.378247543814301E-3</v>
       </c>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J31" s="1">
+        <f t="shared" si="3"/>
+        <v>130.28571428571428</v>
+      </c>
+      <c r="V31" s="13">
+        <v>100</v>
+      </c>
+      <c r="W31" s="1">
+        <v>1.3018867924528301</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B32" s="13">
         <v>100</v>
       </c>
@@ -7156,13 +7346,23 @@
         <f t="shared" si="1"/>
         <v>7.7434805034375942E-3</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="1">
+        <f t="shared" si="3"/>
+        <v>130.18867924528303</v>
+      </c>
+      <c r="V32" s="4">
+        <v>125</v>
+      </c>
+      <c r="W32" s="1">
+        <v>1.0377358490566038</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
         <v>125</v>
       </c>
       <c r="C33" s="4">
-        <f t="shared" ref="C33:C36" si="3">10^-3</f>
+        <f t="shared" ref="C33:C36" si="4">10^-3</f>
         <v>1E-3</v>
       </c>
       <c r="D33" s="5">
@@ -7185,13 +7385,27 @@
         <f t="shared" si="1"/>
         <v>6.7978485062044538E-3</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J33" s="1">
+        <f t="shared" si="3"/>
+        <v>129.71698113207546</v>
+      </c>
+      <c r="L33" s="1">
+        <f>AVERAGE(J15:J36)</f>
+        <v>130.50520800349469</v>
+      </c>
+      <c r="V33" s="4">
+        <v>150</v>
+      </c>
+      <c r="W33" s="1">
+        <v>0.88679245283018859</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
         <v>150</v>
       </c>
       <c r="C34" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
       <c r="D34" s="5">
@@ -7214,13 +7428,23 @@
         <f t="shared" si="1"/>
         <v>6.3045428082680087E-3</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J34" s="1">
+        <f t="shared" si="3"/>
+        <v>133.01886792452828</v>
+      </c>
+      <c r="V34" s="4">
+        <v>200</v>
+      </c>
+      <c r="W34" s="1">
+        <v>0.660377358490566</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
         <v>200</v>
       </c>
       <c r="C35" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
       <c r="D35" s="5">
@@ -7243,13 +7467,23 @@
         <f t="shared" si="1"/>
         <v>5.6527036341048114E-3</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J35" s="1">
+        <f t="shared" si="3"/>
+        <v>132.0754716981132</v>
+      </c>
+      <c r="V35" s="4">
+        <v>500</v>
+      </c>
+      <c r="W35" s="1">
+        <v>0.24761904761904763</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B36" s="4">
         <v>500</v>
       </c>
       <c r="C36" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
       <c r="D36" s="5">
@@ -7272,8 +7506,18 @@
         <f t="shared" si="1"/>
         <v>4.9057215721899187E-3</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J36" s="1">
+        <f t="shared" si="3"/>
+        <v>123.80952380952381</v>
+      </c>
+      <c r="V36" s="4">
+        <v>1000</v>
+      </c>
+      <c r="W36" s="1">
+        <v>0.12307692307692307</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
         <v>1000</v>
       </c>
@@ -7293,11 +7537,11 @@
       <c r="G37" s="4">
         <v>1E-3</v>
       </c>
-      <c r="H37" s="18">
+      <c r="H37" s="15">
         <f t="shared" si="0"/>
         <v>0.12307692307692307</v>
       </c>
-      <c r="I37" s="18">
+      <c r="I37" s="15">
         <f t="shared" si="1"/>
         <v>7.6240858461865027E-4</v>
       </c>
@@ -7314,10 +7558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0024E03-EEC7-4EF9-8387-4BB84283DD59}">
-  <dimension ref="B1:U80"/>
+  <dimension ref="B1:R80"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M69" sqref="M69"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7334,16 +7578,16 @@
     <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -7369,7 +7613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>0.05</v>
       </c>
@@ -7398,7 +7642,7 @@
         <v>7.174241304660875E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>0.1</v>
       </c>
@@ -7427,7 +7671,7 @@
         <v>7.1392262993886665E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>0.25</v>
       </c>
@@ -7456,7 +7700,7 @@
         <v>6.9979805732863387E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
         <v>0.5</v>
       </c>
@@ -7485,7 +7729,7 @@
         <v>7.2094066099958387E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>1</v>
       </c>
@@ -7514,7 +7758,7 @@
         <v>7.102227180806979E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -7543,7 +7787,7 @@
         <v>7.102227180806979E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>5</v>
       </c>
@@ -7572,7 +7816,7 @@
         <v>7.102227180806979E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>8</v>
       </c>
@@ -7601,7 +7845,7 @@
         <v>7.0316435788254306E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>10</v>
       </c>
@@ -7630,7 +7874,7 @@
         <v>6.9801887200106924E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="6">
         <v>12</v>
       </c>
@@ -7659,7 +7903,7 @@
         <v>6.5770977781683004E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>14</v>
       </c>
@@ -7688,7 +7932,7 @@
         <v>6.3611808041148077E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>15</v>
       </c>
@@ -7716,8 +7960,12 @@
         <f t="shared" si="1"/>
         <v>6.2131519274376421E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J16" s="1">
+        <f>H16*B16</f>
+        <v>125.71428571428572</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>16</v>
       </c>
@@ -7745,8 +7993,12 @@
         <f t="shared" si="1"/>
         <v>5.9909718840495993E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J17" s="1">
+        <f t="shared" ref="J17:J31" si="3">H17*B17</f>
+        <v>125.28301886792454</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>18</v>
       </c>
@@ -7774,6 +8026,10 @@
         <f t="shared" si="1"/>
         <v>5.6364729940357829E-2</v>
       </c>
+      <c r="J18" s="1">
+        <f t="shared" si="3"/>
+        <v>124.99999999999999</v>
+      </c>
       <c r="K18" s="2" t="s">
         <v>0</v>
       </c>
@@ -7795,7 +8051,7 @@
         <v>1666666.6666666667</v>
       </c>
     </row>
-    <row r="19" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>20</v>
       </c>
@@ -7823,6 +8079,10 @@
         <f t="shared" si="1"/>
         <v>5.4594798217920154E-2</v>
       </c>
+      <c r="J19" s="1">
+        <f t="shared" si="3"/>
+        <v>125</v>
+      </c>
       <c r="K19" s="2" t="s">
         <v>5</v>
       </c>
@@ -7844,7 +8104,7 @@
         <v>277782.77773277857</v>
       </c>
     </row>
-    <row r="20" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
         <v>25</v>
       </c>
@@ -7872,6 +8132,10 @@
         <f t="shared" si="1"/>
         <v>5.195395439167047E-2</v>
       </c>
+      <c r="J20" s="1">
+        <f t="shared" si="3"/>
+        <v>127.31481481481481</v>
+      </c>
       <c r="Q20" s="2" t="s">
         <v>11</v>
       </c>
@@ -7880,7 +8144,7 @@
         <v>16.666966663966715</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>30</v>
       </c>
@@ -7908,14 +8172,20 @@
         <f t="shared" si="1"/>
         <v>2.0046380189338645E-2</v>
       </c>
-      <c r="T21" s="6">
-        <v>12</v>
-      </c>
-      <c r="U21" s="1">
-        <v>9.7169811320754711</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J21" s="1">
+        <f t="shared" si="3"/>
+        <v>126.38888888888889</v>
+      </c>
+      <c r="P21" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="16">
+        <f>2*10^6</f>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>35</v>
       </c>
@@ -7943,14 +8213,12 @@
         <f t="shared" si="1"/>
         <v>1.8054273102751341E-2</v>
       </c>
-      <c r="T22" s="5">
-        <v>14</v>
-      </c>
-      <c r="U22" s="1">
-        <v>8.8571428571428577</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J22" s="1">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>40</v>
       </c>
@@ -7978,14 +8246,12 @@
         <f t="shared" si="1"/>
         <v>1.6436310916170774E-2</v>
       </c>
-      <c r="T23" s="5">
-        <v>15</v>
-      </c>
-      <c r="U23" s="1">
-        <v>8.3809523809523814</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J23" s="1">
+        <f t="shared" si="3"/>
+        <v>130.76923076923077</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>45</v>
       </c>
@@ -8013,14 +8279,12 @@
         <f t="shared" si="1"/>
         <v>1.4852873985224262E-2</v>
       </c>
-      <c r="T24" s="5">
-        <v>16</v>
-      </c>
-      <c r="U24" s="1">
-        <v>7.8301886792452837</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J24" s="1">
+        <f>H24*B24</f>
+        <v>131.53846153846152</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <v>50</v>
       </c>
@@ -8048,14 +8312,12 @@
         <f t="shared" si="1"/>
         <v>1.3707642470929482E-2</v>
       </c>
-      <c r="T25" s="5">
-        <v>18</v>
-      </c>
-      <c r="U25" s="1">
-        <v>6.9444444444444438</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J25" s="1">
+        <f t="shared" si="3"/>
+        <v>132.03883495145632</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>60</v>
       </c>
@@ -8083,14 +8345,12 @@
         <f t="shared" si="1"/>
         <v>1.1584656144731569E-2</v>
       </c>
-      <c r="T26" s="5">
-        <v>20</v>
-      </c>
-      <c r="U26" s="1">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J26" s="1">
+        <f t="shared" si="3"/>
+        <v>131.53846153846152</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <v>70</v>
       </c>
@@ -8118,14 +8378,16 @@
         <f t="shared" si="1"/>
         <v>1.0257158467720904E-2</v>
       </c>
-      <c r="T27" s="5">
-        <v>25</v>
-      </c>
-      <c r="U27" s="1">
-        <v>5.0925925925925926</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J27" s="1">
+        <f t="shared" si="3"/>
+        <v>131.92307692307693</v>
+      </c>
+      <c r="L27" s="1">
+        <f>AVERAGE(J16:J32)</f>
+        <v>129.53715180645477</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>80</v>
       </c>
@@ -8153,14 +8415,12 @@
         <f t="shared" si="1"/>
         <v>9.1390815729513446E-3</v>
       </c>
-      <c r="T28" s="5">
-        <v>30</v>
-      </c>
-      <c r="U28" s="1">
-        <v>4.2129629629629628</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J28" s="1">
+        <f t="shared" si="3"/>
+        <v>131.04761904761904</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <v>90</v>
       </c>
@@ -8188,14 +8448,12 @@
         <f t="shared" si="1"/>
         <v>8.6671905660192054E-3</v>
       </c>
-      <c r="T29" s="5">
-        <v>35</v>
-      </c>
-      <c r="U29" s="1">
-        <v>3.657142857142857</v>
-      </c>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J29" s="1">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="5">
         <v>100</v>
       </c>
@@ -8223,14 +8481,12 @@
         <f t="shared" si="1"/>
         <v>7.7082375361454715E-3</v>
       </c>
-      <c r="T30" s="5">
-        <v>40</v>
-      </c>
-      <c r="U30" s="1">
-        <v>3.2692307692307692</v>
-      </c>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J30" s="1">
+        <f t="shared" si="3"/>
+        <v>129.24528301886792</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
         <v>125</v>
       </c>
@@ -8258,14 +8514,12 @@
         <f t="shared" si="1"/>
         <v>6.9925633233945761E-3</v>
       </c>
-      <c r="T31" s="5">
-        <v>45</v>
-      </c>
-      <c r="U31" s="1">
-        <v>2.9230769230769229</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="J31" s="1">
+        <f t="shared" si="3"/>
+        <v>136.79245283018867</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>150</v>
       </c>
@@ -8293,14 +8547,8 @@
         <f t="shared" si="1"/>
         <v>6.3639413103327705E-3</v>
       </c>
-      <c r="T32" s="6">
-        <v>50</v>
-      </c>
-      <c r="U32" s="1">
-        <v>2.6407766990291264</v>
-      </c>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="6">
         <v>200</v>
       </c>
@@ -8328,14 +8576,8 @@
         <f t="shared" si="1"/>
         <v>5.8783978002042376E-3</v>
       </c>
-      <c r="T33" s="5">
-        <v>60</v>
-      </c>
-      <c r="U33" s="1">
-        <v>2.1923076923076921</v>
-      </c>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>1000</v>
       </c>
@@ -8362,68 +8604,17 @@
         <f t="shared" si="1"/>
         <v>8.2296369592500687E-4</v>
       </c>
-      <c r="T34" s="6">
-        <v>70</v>
-      </c>
-      <c r="U34" s="1">
-        <v>1.8846153846153846</v>
-      </c>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="T35" s="5">
-        <v>80</v>
-      </c>
-      <c r="U35" s="1">
-        <v>1.638095238095238</v>
-      </c>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="T36" s="6">
-        <v>90</v>
-      </c>
-      <c r="U36" s="1">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="T37" s="5">
-        <v>100</v>
-      </c>
-      <c r="U37" s="1">
-        <v>1.2924528301886793</v>
-      </c>
-    </row>
-    <row r="38" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="T38" s="6">
-        <v>125</v>
-      </c>
-      <c r="U38" s="1">
-        <v>1.0943396226415094</v>
-      </c>
-    </row>
-    <row r="39" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="15" t="s">
+    </row>
+    <row r="38" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="17"/>
-      <c r="T39" s="6">
-        <v>150</v>
-      </c>
-      <c r="U39" s="1">
-        <v>0.90566037735849048</v>
-      </c>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="T40" s="6">
-        <v>200</v>
-      </c>
-      <c r="U40" s="1">
-        <v>0.72380952380952379</v>
-      </c>
-    </row>
-    <row r="41" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="41" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
@@ -8449,7 +8640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
         <v>0.01</v>
       </c>
@@ -8470,15 +8661,15 @@
         <v>0.1</v>
       </c>
       <c r="H42" s="6">
-        <f t="shared" ref="H42:H79" si="3">F42/D42</f>
+        <f t="shared" ref="H42:H79" si="4">F42/D42</f>
         <v>100.98039215686276</v>
       </c>
       <c r="I42" s="6">
-        <f t="shared" ref="I42:I79" si="4">SQRT((G42/D42)^2+(F42/D42^2*E42)^2)</f>
+        <f t="shared" ref="I42:I79" si="5">SQRT((G42/D42)^2+(F42/D42^2*E42)^2)</f>
         <v>0.69664847550782649</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="4">
         <v>0.1</v>
       </c>
@@ -8499,15 +8690,15 @@
         <v>0.1</v>
       </c>
       <c r="H43" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100.98039215686276</v>
       </c>
       <c r="I43" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.69664847550782649</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
         <v>0.2</v>
       </c>
@@ -8528,20 +8719,20 @@
         <v>0.1</v>
       </c>
       <c r="H44" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100.98039215686276</v>
       </c>
       <c r="I44" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.69664847550782649</v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="3">
         <v>1</v>
       </c>
       <c r="C45" s="4">
-        <f t="shared" ref="C45:C53" si="5">1*10^-5</f>
+        <f t="shared" ref="C45:C53" si="6">1*10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D45" s="3">
@@ -8557,20 +8748,20 @@
         <v>0.1</v>
       </c>
       <c r="H45" s="6">
-        <f t="shared" si="3"/>
+        <f>F45/D45</f>
         <v>101.99999999999999</v>
       </c>
       <c r="I45" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.71421285342676377</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="5">
         <v>2</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D46" s="4">
@@ -8586,20 +8777,20 @@
         <v>0.1</v>
       </c>
       <c r="H46" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97.058823529411768</v>
       </c>
       <c r="I46" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.683123283764829</v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="5">
         <v>3</v>
       </c>
       <c r="C47" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D47" s="4">
@@ -8615,20 +8806,20 @@
         <v>0.1</v>
       </c>
       <c r="H47" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.346153846153854</v>
       </c>
       <c r="I47" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.65115608639981237</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="5">
         <v>4</v>
       </c>
       <c r="C48" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D48" s="4">
@@ -8644,11 +8835,11 @@
         <v>0.1</v>
       </c>
       <c r="H48" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87.5</v>
       </c>
       <c r="I48" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.63883087816914963</v>
       </c>
     </row>
@@ -8657,7 +8848,7 @@
         <v>5</v>
       </c>
       <c r="C49" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D49" s="4">
@@ -8673,11 +8864,11 @@
         <v>0.1</v>
       </c>
       <c r="H49" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
       <c r="I49" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.63809229378322341</v>
       </c>
     </row>
@@ -8686,7 +8877,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D50" s="4">
@@ -8702,11 +8893,11 @@
         <v>0.1</v>
       </c>
       <c r="H50" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.961538461538467</v>
       </c>
       <c r="I50" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.60374653386984423</v>
       </c>
     </row>
@@ -8715,7 +8906,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D51" s="4">
@@ -8731,11 +8922,11 @@
         <v>0.1</v>
       </c>
       <c r="H51" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71.15384615384616</v>
       </c>
       <c r="I51" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.59005232565121501</v>
       </c>
     </row>
@@ -8744,7 +8935,7 @@
         <v>8</v>
       </c>
       <c r="C52" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D52" s="4">
@@ -8760,11 +8951,11 @@
         <v>0.1</v>
       </c>
       <c r="H52" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.346153846153854</v>
       </c>
       <c r="I52" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.57695937646575346</v>
       </c>
     </row>
@@ -8773,7 +8964,7 @@
         <v>9</v>
       </c>
       <c r="C53" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D53" s="4">
@@ -8789,11 +8980,11 @@
         <v>0.1</v>
       </c>
       <c r="H53" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61.538461538461547</v>
       </c>
       <c r="I53" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.56450952376012387</v>
       </c>
     </row>
@@ -8802,7 +8993,7 @@
         <v>10</v>
       </c>
       <c r="C54" s="4">
-        <f t="shared" ref="C54:C72" si="6">10^-4</f>
+        <f t="shared" ref="C54:C72" si="7">10^-4</f>
         <v>1E-4</v>
       </c>
       <c r="D54" s="4">
@@ -8818,11 +9009,11 @@
         <v>0.1</v>
       </c>
       <c r="H54" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>57.692307692307693</v>
       </c>
       <c r="I54" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.55504182765545995</v>
       </c>
     </row>
@@ -8831,7 +9022,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D55" s="4">
@@ -8847,11 +9038,11 @@
         <v>0.1</v>
       </c>
       <c r="H55" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53.846153846153847</v>
       </c>
       <c r="I55" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.54603635577786247</v>
       </c>
       <c r="K55" s="2" t="s">
@@ -8880,7 +9071,7 @@
         <v>12</v>
       </c>
       <c r="C56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D56" s="4">
@@ -8896,11 +9087,11 @@
         <v>0.1</v>
       </c>
       <c r="H56" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50.000000000000007</v>
       </c>
       <c r="I56" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.53751634074514176</v>
       </c>
       <c r="K56" s="2" t="s">
@@ -8929,7 +9120,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D57" s="4">
@@ -8945,11 +9136,11 @@
         <v>0.01</v>
       </c>
       <c r="H57" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47.11538461538462</v>
       </c>
       <c r="I57" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.23156211283174907</v>
       </c>
       <c r="Q57" s="2" t="s">
@@ -8965,7 +9156,7 @@
         <v>14</v>
       </c>
       <c r="C58" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D58" s="4">
@@ -8981,11 +9172,11 @@
         <v>0.01</v>
       </c>
       <c r="H58" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44.230769230769226</v>
       </c>
       <c r="I58" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.21801498168249098</v>
       </c>
     </row>
@@ -8994,7 +9185,7 @@
         <v>15</v>
       </c>
       <c r="C59" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D59" s="4">
@@ -9010,12 +9201,16 @@
         <v>0.01</v>
       </c>
       <c r="H59" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>42.307692307692314</v>
       </c>
       <c r="I59" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.20900696968853244</v>
+      </c>
+      <c r="J59" s="1">
+        <f>H59*B59</f>
+        <v>634.61538461538476</v>
       </c>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.3">
@@ -9023,7 +9218,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D60" s="4">
@@ -9039,12 +9234,16 @@
         <v>0.01</v>
       </c>
       <c r="H60" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38.942307692307693</v>
       </c>
       <c r="I60" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.19329693450998411</v>
+      </c>
+      <c r="J60" s="1">
+        <f>H60*B60</f>
+        <v>623.07692307692309</v>
       </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.3">
@@ -9052,7 +9251,7 @@
         <v>17</v>
       </c>
       <c r="C61" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D61" s="4">
@@ -9068,12 +9267,16 @@
         <v>0.01</v>
       </c>
       <c r="H61" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
       <c r="I61" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.18658863817620225</v>
+      </c>
+      <c r="J61" s="1">
+        <f>H61*B61</f>
+        <v>637.5</v>
       </c>
     </row>
     <row r="62" spans="2:18" x14ac:dyDescent="0.3">
@@ -9081,7 +9284,7 @@
         <v>18</v>
       </c>
       <c r="C62" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D62" s="4">
@@ -9097,12 +9300,16 @@
         <v>0.01</v>
       </c>
       <c r="H62" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35.769230769230774</v>
       </c>
       <c r="I62" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.17856146371882367</v>
+      </c>
+      <c r="J62" s="1">
+        <f>H62*B62</f>
+        <v>643.84615384615392</v>
       </c>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.3">
@@ -9110,7 +9317,7 @@
         <v>19</v>
       </c>
       <c r="C63" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D63" s="4">
@@ -9126,12 +9333,16 @@
         <v>0.01</v>
       </c>
       <c r="H63" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33.846153846153847</v>
       </c>
       <c r="I63" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.16967558797269913</v>
+      </c>
+      <c r="J63" s="1">
+        <f>H63*B63</f>
+        <v>643.07692307692309</v>
       </c>
     </row>
     <row r="64" spans="2:18" x14ac:dyDescent="0.3">
@@ -9139,7 +9350,7 @@
         <v>20</v>
       </c>
       <c r="C64" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D64" s="4">
@@ -9155,20 +9366,24 @@
         <v>0.01</v>
       </c>
       <c r="H64" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32.692307692307693</v>
       </c>
       <c r="I64" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.16436310916170777</v>
       </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J64" s="1">
+        <f>H64*B64</f>
+        <v>653.84615384615381</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
         <v>25</v>
       </c>
       <c r="C65" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D65" s="4">
@@ -9184,20 +9399,24 @@
         <v>0.01</v>
       </c>
       <c r="H65" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26.037735849056602</v>
       </c>
       <c r="I65" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.13156603977752185</v>
       </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J65" s="1">
+        <f>H65*B65</f>
+        <v>650.94339622641508</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="6">
         <v>30</v>
       </c>
       <c r="C66" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D66" s="4">
@@ -9213,20 +9432,24 @@
         <v>0.01</v>
       </c>
       <c r="H66" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.815533980582526</v>
       </c>
       <c r="I66" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.1209262753834764</v>
       </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J66" s="1">
+        <f>H66*B66</f>
+        <v>684.46601941747576</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="6">
         <v>40</v>
       </c>
       <c r="C67" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D67" s="4">
@@ -9242,20 +9465,24 @@
         <v>0.01</v>
       </c>
       <c r="H67" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17.30769230769231</v>
       </c>
       <c r="I67" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.610049156942517E-2</v>
       </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J67" s="1">
+        <f>H67*B67</f>
+        <v>692.30769230769238</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B68" s="6">
         <v>50</v>
       </c>
       <c r="C68" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D68" s="4">
@@ -9271,20 +9498,28 @@
         <v>0.01</v>
       </c>
       <c r="H68" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.230769230769232</v>
       </c>
       <c r="I68" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3619963421560764E-2</v>
       </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J68" s="1">
+        <f>H68*B68</f>
+        <v>711.53846153846155</v>
+      </c>
+      <c r="L68" s="1">
+        <f>AVERAGE(J59:J79)</f>
+        <v>697.10858464221212</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" s="4">
         <v>60</v>
       </c>
       <c r="C69" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D69" s="4">
@@ -9300,20 +9535,24 @@
         <v>0.01</v>
       </c>
       <c r="H69" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.923076923076923</v>
       </c>
       <c r="I69" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.4814823683964166E-2</v>
       </c>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J69" s="1">
+        <f>H69*B69</f>
+        <v>715.38461538461536</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
         <v>70</v>
       </c>
       <c r="C70" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D70" s="4">
@@ -9329,20 +9568,24 @@
         <v>0.01</v>
       </c>
       <c r="H70" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.188679245283019</v>
       </c>
       <c r="I70" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.7340450117575459E-2</v>
       </c>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J70" s="1">
+        <f>H70*B70</f>
+        <v>713.20754716981139</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="4">
         <v>80</v>
       </c>
       <c r="C71" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D71" s="4">
@@ -9358,20 +9601,24 @@
         <v>0.01</v>
       </c>
       <c r="H71" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.433962264150944</v>
       </c>
       <c r="I71" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.4847708194898088E-2</v>
       </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J71" s="1">
+        <f>H71*B71</f>
+        <v>754.71698113207549</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B72" s="4">
         <v>90</v>
       </c>
       <c r="C72" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
       <c r="D72" s="4">
@@ -9387,20 +9634,24 @@
         <v>0.01</v>
       </c>
       <c r="H72" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.9245283018867925</v>
       </c>
       <c r="I72" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.0185083882864768E-2</v>
       </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J72" s="1">
+        <f>H72*B72</f>
+        <v>713.20754716981128</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="4">
         <v>100</v>
       </c>
       <c r="C73" s="4">
-        <f t="shared" ref="C73:C79" si="7">10^-3</f>
+        <f t="shared" ref="C73:C79" si="8">10^-3</f>
         <v>1E-3</v>
       </c>
       <c r="D73" s="4">
@@ -9416,20 +9667,24 @@
         <v>0.01</v>
       </c>
       <c r="H73" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.5471698113207557</v>
       </c>
       <c r="I73" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.9096031687554396E-2</v>
       </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J73" s="1">
+        <f>H73*B73</f>
+        <v>754.7169811320756</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B74" s="4">
         <v>150</v>
       </c>
       <c r="C74" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1E-3</v>
       </c>
       <c r="D74" s="4">
@@ -9445,20 +9700,24 @@
         <v>0.01</v>
       </c>
       <c r="H74" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.6603773584905657</v>
       </c>
       <c r="I74" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.4202171515076947E-2</v>
       </c>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J74" s="1">
+        <f>H74*B74</f>
+        <v>849.05660377358481</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="4">
         <v>200</v>
       </c>
       <c r="C75" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1E-3</v>
       </c>
       <c r="D75" s="4">
@@ -9474,20 +9733,24 @@
         <v>1E-3</v>
       </c>
       <c r="H75" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4615384615384617</v>
       </c>
       <c r="I75" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.7322542054186936E-2</v>
       </c>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J75" s="1">
+        <f>H75*B75</f>
+        <v>692.30769230769238</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B76" s="4">
         <v>300</v>
       </c>
       <c r="C76" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1E-3</v>
       </c>
       <c r="D76" s="4">
@@ -9503,20 +9766,24 @@
         <v>1E-3</v>
       </c>
       <c r="H76" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3461538461538463</v>
       </c>
       <c r="I76" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2261442048890833E-2</v>
       </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J76" s="1">
+        <f>H76*B76</f>
+        <v>703.84615384615392</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="4">
         <v>400</v>
       </c>
       <c r="C77" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1E-3</v>
       </c>
       <c r="D77" s="4">
@@ -9532,20 +9799,24 @@
         <v>1E-3</v>
       </c>
       <c r="H77" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7523809523809524</v>
       </c>
       <c r="I77" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.6077715640951918E-3</v>
       </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J77" s="1">
+        <f>H77*B77</f>
+        <v>700.95238095238096</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="4">
         <v>500</v>
       </c>
       <c r="C78" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1E-3</v>
       </c>
       <c r="D78" s="4">
@@ -9561,20 +9832,24 @@
         <v>1E-3</v>
       </c>
       <c r="H78" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4095238095238094</v>
       </c>
       <c r="I78" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.2296369592500685E-3</v>
       </c>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J78" s="1">
+        <f>H78*B78</f>
+        <v>704.7619047619047</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="4">
         <v>1000</v>
       </c>
       <c r="C79" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1E-3</v>
       </c>
       <c r="D79" s="4">
@@ -9590,24 +9865,29 @@
         <v>1E-3</v>
       </c>
       <c r="H79" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.76190476190476197</v>
       </c>
       <c r="I79" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.9865663412444836E-3</v>
       </c>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J79" s="1">
+        <f>H79*B79</f>
+        <v>761.90476190476193</v>
+      </c>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
       <c r="I80" s="14"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:I34">
     <sortCondition ref="B5:B34"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B39:E39"/>
+    <mergeCell ref="P21:Q21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>